<commit_message>
Fixed database class data reading
</commit_message>
<xml_diff>
--- a/RohrleitungsGenerator/Resources/database.xlsx
+++ b/RohrleitungsGenerator/Resources/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maxim Stötzer\Studium\6. Semester\CAD 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfp\source\repos\RohrleitungsGenerator\RohrleitungsGenerator\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E3B7463-8638-4BFF-A105-F8567F0FC362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBE00F4-C4D0-4FD0-8FE4-B62FC703E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="22230" windowHeight="15600" xr2:uid="{40B27918-9E70-4D90-BE77-B8C8655450F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{40B27918-9E70-4D90-BE77-B8C8655450F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Normrohre" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Wandstärke</t>
   </si>
@@ -135,84 +135,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Biegewiderstandsmoment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in []</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Torsionswiderstandsmoment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in []</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Querschnittsfläche</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in []</t>
-    </r>
-  </si>
-  <si>
-    <t>I=64π​(D^4−d^4)</t>
-  </si>
-  <si>
-    <t>J=32π​(D^4−d^4)</t>
-  </si>
-  <si>
-    <t>A=4π​(D^2−d^2)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>E-Modu</t>
     </r>
     <r>
@@ -491,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,8 +426,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -548,11 +476,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -567,6 +510,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -579,23 +531,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -939,7 +885,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,219 +908,219 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C21" s="5">
         <v>1067</v>
@@ -1182,10 +1128,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C22" s="5">
         <v>1219</v>
@@ -1193,10 +1139,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" s="5">
         <v>1371</v>
@@ -1204,10 +1150,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C24" s="5">
         <v>1524</v>
@@ -1215,10 +1161,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C25" s="5">
         <v>1829</v>
@@ -1330,7 +1276,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E3" sqref="E3:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,55 +1294,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>16</v>
+      <c r="D1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="11">
         <f>210*10^9</f>
         <v>210000000000</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="11">
         <f>12*10^-6</f>
         <v>1.2E-5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="11">
         <f>400*10^6</f>
         <v>400000000</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="11">
         <v>7850</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="11">
         <f>81*10^9</f>
         <v>81000000000</v>
       </c>
@@ -1404,93 +1350,92 @@
       <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="11">
         <f>2.4*10^9</f>
         <v>2400000000</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="11">
         <f>65*10^-6</f>
         <v>6.4999999999999994E-5</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <f>65*10^6</f>
         <v>65000000</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="11">
         <v>1200</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="11">
         <f>1*10^9</f>
         <v>1000000000</v>
       </c>
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="Q6" s="3"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E3:E4"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
@@ -1501,23 +1446,12 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1528,7 +1462,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,20 +1472,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>15</v>
+      <c r="B1" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -1559,7 +1493,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>870</v>
@@ -1567,7 +1501,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1.2</v>

</xml_diff>